<commit_message>
More complete transformer specs
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/patient_import_test.xlsx
+++ b/spec/fixtures/files/patient_import_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hariharanmohanraj/code/simple/simple-server/spec/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63AFCF6-F8BF-2C48-83F8-B70E31C4933E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D33F806-6865-2C41-BD82-D97AE66BAE5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="2300" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="patient-list_facility_group_Sri" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,23 @@
     <sheet name="common medicines" sheetId="3" r:id="rId3"/>
     <sheet name="regions" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="131">
   <si>
     <t>registration_facility</t>
   </si>
@@ -119,9 +130,6 @@
   </si>
   <si>
     <t>Addishiwot Health Center</t>
-  </si>
-  <si>
-    <t>Example Patient</t>
   </si>
   <si>
     <t>Male</t>
@@ -265,18 +273,6 @@
     <t>Captopril 25 mg TID</t>
   </si>
   <si>
-    <t>Enalpril 5 mg</t>
-  </si>
-  <si>
-    <t>Enalpril 10 mg</t>
-  </si>
-  <si>
-    <t>Enalpril 20 mg</t>
-  </si>
-  <si>
-    <t>Enalpril 40 mg</t>
-  </si>
-  <si>
     <t>Glibenclamide 2.5 mg PD</t>
   </si>
   <si>
@@ -392,6 +388,45 @@
   </si>
   <si>
     <t>first_visit_medication_5</t>
+  </si>
+  <si>
+    <t>No Meds In Last Visit</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>0000002</t>
+  </si>
+  <si>
+    <t>Basic Patient 1</t>
+  </si>
+  <si>
+    <t>Basic Patient 2</t>
+  </si>
+  <si>
+    <t>0000003</t>
+  </si>
+  <si>
+    <t>56 Side Street</t>
+  </si>
+  <si>
+    <t>No Last Visit</t>
+  </si>
+  <si>
+    <t>0000004</t>
+  </si>
+  <si>
+    <t>Enalapril 5 mg</t>
+  </si>
+  <si>
+    <t>Enalapril 10 mg</t>
+  </si>
+  <si>
+    <t>Enalapril 20 mg</t>
+  </si>
+  <si>
+    <t>Enalapril 40 mg</t>
   </si>
 </sst>
 </file>
@@ -530,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -552,6 +587,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -767,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BB500"/>
+  <dimension ref="A1:BB502"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -872,19 +908,19 @@
         <v>20</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="AA1" s="4" t="s">
         <v>21</v>
@@ -1055,52 +1091,52 @@
         <v>44120.393055555556</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>32</v>
+        <v>121</v>
       </c>
       <c r="D3" s="12">
         <v>45</v>
       </c>
       <c r="E3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="G3" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="H3" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>36</v>
       </c>
       <c r="I3" s="12">
         <v>936528787</v>
       </c>
       <c r="J3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="L3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="M3" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="N3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="O3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>42</v>
-      </c>
       <c r="Q3" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R3" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S3" s="13">
         <v>43859</v>
@@ -1112,19 +1148,19 @@
         <v>90</v>
       </c>
       <c r="V3" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="W3" s="12" t="s">
-        <v>79</v>
+        <v>127</v>
       </c>
       <c r="X3" s="12" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="Y3" s="12" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="Z3" s="12" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="AA3" s="13">
         <v>44251</v>
@@ -1136,19 +1172,19 @@
         <v>89</v>
       </c>
       <c r="AD3" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AE3" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AF3" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AG3" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AH3" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI3" s="18"/>
       <c r="AJ3" s="18"/>
@@ -1159,89 +1195,324 @@
       <c r="AO3" s="18"/>
     </row>
     <row r="4" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="12"/>
-      <c r="AA4" s="13"/>
-      <c r="AB4" s="17"/>
-      <c r="AC4" s="17"/>
-      <c r="AD4" s="12"/>
-      <c r="AE4" s="12"/>
-      <c r="AF4" s="12"/>
-      <c r="AG4" s="12"/>
-      <c r="AH4" s="12"/>
+      <c r="A4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="13">
+        <v>44185.393055555556</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="12">
+        <v>56</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="12">
+        <v>927485753</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="R4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="13">
+        <v>43859</v>
+      </c>
+      <c r="T4" s="17">
+        <v>160</v>
+      </c>
+      <c r="U4" s="17">
+        <v>90</v>
+      </c>
+      <c r="V4" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="W4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="X4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA4" s="13">
+        <v>44251</v>
+      </c>
+      <c r="AB4" s="17">
+        <v>145</v>
+      </c>
+      <c r="AC4" s="17">
+        <v>89</v>
+      </c>
+      <c r="AD4" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI4" s="18"/>
+      <c r="AJ4" s="18"/>
+      <c r="AK4" s="18"/>
+      <c r="AL4" s="18"/>
+      <c r="AM4" s="18"/>
+      <c r="AN4" s="18"/>
+      <c r="AO4" s="18"/>
     </row>
     <row r="5" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="17"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="12"/>
+      <c r="A5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="13">
+        <v>44120.393055555556</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="12">
+        <v>45</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" s="12">
+        <v>936528787</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="R5" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="S5" s="13">
+        <v>43859</v>
+      </c>
+      <c r="T5" s="17">
+        <v>160</v>
+      </c>
+      <c r="U5" s="17">
+        <v>90</v>
+      </c>
+      <c r="V5" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="W5" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="X5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z5" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="AA5" s="13"/>
       <c r="AB5" s="17"/>
       <c r="AC5" s="17"/>
-      <c r="AD5" s="12"/>
-      <c r="AE5" s="12"/>
-      <c r="AF5" s="12"/>
-      <c r="AG5" s="12"/>
-      <c r="AH5" s="12"/>
+      <c r="AD5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI5" s="18"/>
+      <c r="AJ5" s="18"/>
+      <c r="AK5" s="18"/>
+      <c r="AL5" s="18"/>
+      <c r="AM5" s="18"/>
+      <c r="AN5" s="18"/>
+      <c r="AO5" s="18"/>
     </row>
     <row r="6" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="12"/>
-      <c r="AA6" s="13"/>
-      <c r="AB6" s="17"/>
-      <c r="AC6" s="17"/>
-      <c r="AD6" s="12"/>
-      <c r="AE6" s="12"/>
-      <c r="AF6" s="12"/>
-      <c r="AG6" s="12"/>
-      <c r="AH6" s="12"/>
+      <c r="A6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="13">
+        <v>44120.393055555556</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="12">
+        <v>56</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6" s="12">
+        <v>936528787</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="R6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="S6" s="13">
+        <v>43859</v>
+      </c>
+      <c r="T6" s="17">
+        <v>160</v>
+      </c>
+      <c r="U6" s="17">
+        <v>90</v>
+      </c>
+      <c r="V6" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="W6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="X6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA6" s="13">
+        <v>44251</v>
+      </c>
+      <c r="AB6" s="17">
+        <v>145</v>
+      </c>
+      <c r="AC6" s="17">
+        <v>89</v>
+      </c>
+      <c r="AD6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH6" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="7" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
@@ -15075,18 +15346,74 @@
       <c r="AG500" s="12"/>
       <c r="AH500" s="12"/>
     </row>
+    <row r="501" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A501" s="12"/>
+      <c r="B501" s="13"/>
+      <c r="F501" s="14"/>
+      <c r="G501" s="16"/>
+      <c r="H501" s="16"/>
+      <c r="M501" s="12"/>
+      <c r="N501" s="12"/>
+      <c r="O501" s="12"/>
+      <c r="P501" s="12"/>
+      <c r="Q501" s="12"/>
+      <c r="R501" s="12"/>
+      <c r="T501" s="17"/>
+      <c r="U501" s="17"/>
+      <c r="V501" s="12"/>
+      <c r="W501" s="12"/>
+      <c r="X501" s="12"/>
+      <c r="Y501" s="12"/>
+      <c r="Z501" s="12"/>
+      <c r="AA501" s="13"/>
+      <c r="AB501" s="17"/>
+      <c r="AC501" s="17"/>
+      <c r="AD501" s="12"/>
+      <c r="AE501" s="12"/>
+      <c r="AF501" s="12"/>
+      <c r="AG501" s="12"/>
+      <c r="AH501" s="12"/>
+    </row>
+    <row r="502" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A502" s="12"/>
+      <c r="B502" s="13"/>
+      <c r="F502" s="14"/>
+      <c r="G502" s="16"/>
+      <c r="H502" s="16"/>
+      <c r="M502" s="12"/>
+      <c r="N502" s="12"/>
+      <c r="O502" s="12"/>
+      <c r="P502" s="12"/>
+      <c r="Q502" s="12"/>
+      <c r="R502" s="12"/>
+      <c r="T502" s="17"/>
+      <c r="U502" s="17"/>
+      <c r="V502" s="12"/>
+      <c r="W502" s="12"/>
+      <c r="X502" s="12"/>
+      <c r="Y502" s="12"/>
+      <c r="Z502" s="12"/>
+      <c r="AA502" s="13"/>
+      <c r="AB502" s="17"/>
+      <c r="AC502" s="17"/>
+      <c r="AD502" s="12"/>
+      <c r="AE502" s="12"/>
+      <c r="AF502" s="12"/>
+      <c r="AG502" s="12"/>
+      <c r="AH502" s="12"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AB4:AB500" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AB7:AB502" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Amlodipine,Aspirin,Captopril,Enalpril,Glibenclamide,Glimeperide,Hydrochlorothiazide,Lisinopril,Metformin,Metoprolol,Propranolol"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N3:R500" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N3:R502" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"yes,no,unknown"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E4" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Male,Female"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F3:F500" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F3:F502" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
@@ -15099,19 +15426,19 @@
           <x14:formula1>
             <xm:f>regions!$A$1:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M500</xm:sqref>
+          <xm:sqref>M3:M502</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>'facility names'!$A$1:$A$100</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A500</xm:sqref>
+          <xm:sqref>A3:A502</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>'common medicines'!$A$1:$A$40</xm:f>
           </x14:formula1>
-          <xm:sqref>V3:Z3 U4:Z500 AD3:AH500</xm:sqref>
+          <xm:sqref>U7:Z502 V3:Z6 AD3:AH502</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -15138,157 +15465,157 @@
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16269,7 +16596,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16279,172 +16608,172 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>83</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17433,62 +17762,62 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Do not include rxnorm code if it is not available
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/patient_import_test.xlsx
+++ b/spec/fixtures/files/patient_import_test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hariharanmohanraj/code/simple/simple-server/spec/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F53763-F30F-7E4D-9E69-CE78DB1AC4C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F64E6BE-0D9D-6547-944E-F92CD8C2BA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="133">
   <si>
     <t>registration_date</t>
   </si>
@@ -428,6 +428,12 @@
   <si>
     <t>Vegetable District</t>
   </si>
+  <si>
+    <t>No Rxnorm Code</t>
+  </si>
+  <si>
+    <t>0000005</t>
+  </si>
 </sst>
 </file>
 
@@ -815,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BA502"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:S1048576"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1505,23 +1511,81 @@
       </c>
     </row>
     <row r="7" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="12"/>
+      <c r="A7" s="13">
+        <v>44120.393055555556</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="14">
+        <v>67</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="H7" s="14">
+        <v>935234938</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="S7" s="17">
+        <v>160</v>
+      </c>
+      <c r="T7" s="17">
+        <v>90</v>
+      </c>
+      <c r="U7" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="V7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="W7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="X7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y7" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="Z7" s="13"/>
       <c r="AA7" s="17"/>
       <c r="AB7" s="17"/>
@@ -14926,7 +14990,7 @@
           <x14:formula1>
             <xm:f>'common medicines'!$A$1:$A$40</xm:f>
           </x14:formula1>
-          <xm:sqref>T7:Y502 U3:Y6 AC3:AG502</xm:sqref>
+          <xm:sqref>AC3:AG502 U3:Y6 U7:Y502 T35:T502</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Do not include rxnorm code if it is not available (#2527)
**Story card:** [ch3545](https://app.clubhouse.io/simpledotorg/story/3545/missing-rxnorm-code-fix)

## Because

Some medications in our canonical list do not have an RxNorm code. When one of these medications is included in an import file, a validation error is thrown. 

## This addresses

Strip `rxnorm` from the params payload if it is missing. The param is optional in our API anyway. It just cannot be `nil`.
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/patient_import_test.xlsx
+++ b/spec/fixtures/files/patient_import_test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hariharanmohanraj/code/simple/simple-server/spec/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F53763-F30F-7E4D-9E69-CE78DB1AC4C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F64E6BE-0D9D-6547-944E-F92CD8C2BA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="133">
   <si>
     <t>registration_date</t>
   </si>
@@ -428,6 +428,12 @@
   <si>
     <t>Vegetable District</t>
   </si>
+  <si>
+    <t>No Rxnorm Code</t>
+  </si>
+  <si>
+    <t>0000005</t>
+  </si>
 </sst>
 </file>
 
@@ -815,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BA502"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:S1048576"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1505,23 +1511,81 @@
       </c>
     </row>
     <row r="7" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="12"/>
+      <c r="A7" s="13">
+        <v>44120.393055555556</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="14">
+        <v>67</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="H7" s="14">
+        <v>935234938</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="S7" s="17">
+        <v>160</v>
+      </c>
+      <c r="T7" s="17">
+        <v>90</v>
+      </c>
+      <c r="U7" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="V7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="W7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="X7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y7" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="Z7" s="13"/>
       <c r="AA7" s="17"/>
       <c r="AB7" s="17"/>
@@ -14926,7 +14990,7 @@
           <x14:formula1>
             <xm:f>'common medicines'!$A$1:$A$40</xm:f>
           </x14:formula1>
-          <xm:sqref>T7:Y502 U3:Y6 AC3:AG502</xm:sqref>
+          <xm:sqref>AC3:AG502 U3:Y6 U7:Y502 T35:T502</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Mark missing history questions as "unknown"
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/patient_import_test.xlsx
+++ b/spec/fixtures/files/patient_import_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hariharanmohanraj/code/simple/simple-server/spec/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F64E6BE-0D9D-6547-944E-F92CD8C2BA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC78976C-9F1E-8E41-81EE-59F1BAA46A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="133">
   <si>
     <t>registration_date</t>
   </si>
@@ -821,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BA502"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1137,9 +1137,7 @@
       <c r="O3" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="12" t="s">
-        <v>39</v>
-      </c>
+      <c r="P3" s="12"/>
       <c r="Q3" s="12" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Recognize Y/N for Died?
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/patient_import_test.xlsx
+++ b/spec/fixtures/files/patient_import_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hariharanmohanraj/code/simple/simple-server/spec/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B60E27B-A64E-9C4C-B8AD-2484A605F202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B692A30-B815-7C48-9D7A-2D2294A5E5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="148">
   <si>
     <t>registration_date</t>
   </si>
@@ -461,6 +461,24 @@
   <si>
     <t>0000008</t>
   </si>
+  <si>
+    <t>Died Abbrev Y</t>
+  </si>
+  <si>
+    <t>Died Abbrev N</t>
+  </si>
+  <si>
+    <t>0000009</t>
+  </si>
+  <si>
+    <t>0000010</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
 </sst>
 </file>
 
@@ -849,7 +867,7 @@
   <dimension ref="A1:BA502"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E12" sqref="E11:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1876,60 +1894,204 @@
       <c r="AG10" s="12"/>
     </row>
     <row r="11" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
+      <c r="A11" s="13">
+        <v>44120.393055555556</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="12">
+        <v>45</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="H11" s="12">
+        <v>936528787</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="N11" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="O11" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="12"/>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="17"/>
-      <c r="AB11" s="17"/>
-      <c r="AC11" s="12"/>
-      <c r="AD11" s="12"/>
-      <c r="AE11" s="12"/>
-      <c r="AF11" s="12"/>
-      <c r="AG11" s="12"/>
+      <c r="Q11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="R11" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="S11" s="17">
+        <v>160</v>
+      </c>
+      <c r="T11" s="17">
+        <v>90</v>
+      </c>
+      <c r="U11" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="V11" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="W11" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="X11" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y11" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z11" s="13">
+        <v>44251</v>
+      </c>
+      <c r="AA11" s="17">
+        <v>145</v>
+      </c>
+      <c r="AB11" s="17">
+        <v>89</v>
+      </c>
+      <c r="AC11" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG11" s="12" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="17"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="12"/>
-      <c r="Y12" s="12"/>
-      <c r="Z12" s="13"/>
-      <c r="AA12" s="17"/>
-      <c r="AB12" s="17"/>
-      <c r="AC12" s="12"/>
-      <c r="AD12" s="12"/>
-      <c r="AE12" s="12"/>
-      <c r="AF12" s="12"/>
-      <c r="AG12" s="12"/>
+      <c r="A12" s="13">
+        <v>44185.393055555556</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="12">
+        <v>56</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" t="s">
+        <v>147</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="H12" s="12">
+        <v>927485753</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="P12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q12" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="R12" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="S12" s="17">
+        <v>160</v>
+      </c>
+      <c r="T12" s="17">
+        <v>90</v>
+      </c>
+      <c r="U12" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="V12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="W12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="X12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z12" s="13">
+        <v>44251</v>
+      </c>
+      <c r="AA12" s="17">
+        <v>145</v>
+      </c>
+      <c r="AB12" s="17">
+        <v>89</v>
+      </c>
+      <c r="AC12" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG12" s="12" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="13" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
@@ -15163,13 +15325,13 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AA7:AA502" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AA7:AA10 AA13:AA502" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Amlodipine,Aspirin,Captopril,Enalpril,Glibenclamide,Glimeperide,Hydrochlorothiazide,Lisinopril,Metformin,Metoprolol,Propranolol"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N3:R502" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"yes,no,unknown"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D3:D6" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D3:D6 D11:D12" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Male,Female"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E502" xr:uid="{00000000-0002-0000-0000-000006000000}">
@@ -15191,7 +15353,7 @@
           <x14:formula1>
             <xm:f>'common medicines'!$A$1:$A$40</xm:f>
           </x14:formula1>
-          <xm:sqref>AC3:AG502 T35:T502 U3:Y502</xm:sqref>
+          <xm:sqref>T35:T502 AC3:AG502 U3:Y502</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
More exhaustive test cases
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/patient_import_test.xlsx
+++ b/spec/fixtures/files/patient_import_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hariharanmohanraj/code/simple/simple-server/spec/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B692A30-B815-7C48-9D7A-2D2294A5E5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FD6B2E-2BA8-214C-8159-306D68BCE5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="154">
   <si>
     <t>registration_date</t>
   </si>
@@ -479,6 +479,24 @@
   <si>
     <t>N</t>
   </si>
+  <si>
+    <t>0000011</t>
+  </si>
+  <si>
+    <t>Random Gender</t>
+  </si>
+  <si>
+    <t>Died Abbrev Random</t>
+  </si>
+  <si>
+    <t>0000012</t>
+  </si>
+  <si>
+    <t>Potato</t>
+  </si>
+  <si>
+    <t>Random gender</t>
+  </si>
 </sst>
 </file>
 
@@ -864,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BA502"/>
+  <dimension ref="A1:BA503"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="E12" sqref="E11:E12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1897,17 +1915,17 @@
       <c r="A11" s="13">
         <v>44120.393055555556</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="C11" s="12">
-        <v>45</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>146</v>
+      <c r="B11" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="14">
+        <v>67</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>31</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>32</v>
@@ -1939,7 +1957,9 @@
       <c r="O11" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="P11" s="12"/>
+      <c r="P11" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="Q11" s="12" t="s">
         <v>31</v>
       </c>
@@ -1953,60 +1973,44 @@
         <v>90</v>
       </c>
       <c r="U11" s="12" t="s">
-        <v>72</v>
+        <v>128</v>
       </c>
       <c r="V11" s="12" t="s">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="W11" s="12" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="X11" s="12" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="Y11" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z11" s="13">
-        <v>44251</v>
-      </c>
-      <c r="AA11" s="17">
-        <v>145</v>
-      </c>
-      <c r="AB11" s="17">
-        <v>89</v>
-      </c>
-      <c r="AC11" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD11" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="AE11" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF11" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG11" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="17"/>
+      <c r="AB11" s="17"/>
+      <c r="AC11" s="12"/>
+      <c r="AD11" s="12"/>
+      <c r="AE11" s="12"/>
+      <c r="AF11" s="12"/>
+      <c r="AG11" s="12"/>
     </row>
     <row r="12" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
-        <v>44185.393055555556</v>
+        <v>44120.393055555556</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C12" s="12">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>32</v>
@@ -2015,10 +2019,10 @@
         <v>145</v>
       </c>
       <c r="H12" s="12">
-        <v>927485753</v>
+        <v>936528787</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>122</v>
+        <v>34</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>35</v>
@@ -2033,19 +2037,17 @@
         <v>37</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O12" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="R12" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="P12" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q12" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="R12" s="12" t="s">
-        <v>31</v>
       </c>
       <c r="S12" s="17">
         <v>160</v>
@@ -2057,16 +2059,16 @@
         <v>72</v>
       </c>
       <c r="V12" s="12" t="s">
-        <v>40</v>
+        <v>125</v>
       </c>
       <c r="W12" s="12" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="X12" s="12" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="Y12" s="12" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="Z12" s="13">
         <v>44251</v>
@@ -2094,43 +2096,161 @@
       </c>
     </row>
     <row r="13" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="17"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="12"/>
-      <c r="Z13" s="13"/>
-      <c r="AA13" s="17"/>
-      <c r="AB13" s="17"/>
-      <c r="AC13" s="12"/>
-      <c r="AD13" s="12"/>
-      <c r="AE13" s="12"/>
-      <c r="AF13" s="12"/>
-      <c r="AG13" s="12"/>
+      <c r="A13" s="13">
+        <v>44185.393055555556</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="12">
+        <v>56</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E13" t="s">
+        <v>147</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H13" s="12">
+        <v>927485753</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="O13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="P13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="R13" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="S13" s="17">
+        <v>160</v>
+      </c>
+      <c r="T13" s="17">
+        <v>90</v>
+      </c>
+      <c r="U13" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="V13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="W13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="X13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z13" s="13">
+        <v>44251</v>
+      </c>
+      <c r="AA13" s="17">
+        <v>145</v>
+      </c>
+      <c r="AB13" s="17">
+        <v>89</v>
+      </c>
+      <c r="AC13" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG13" s="12" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
+      <c r="A14" s="13">
+        <v>44185.393055555556</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" s="12">
+        <v>56</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="H14" s="12">
+        <v>927485753</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="O14" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="P14" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q14" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="R14" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="S14" s="17"/>
       <c r="T14" s="17"/>
       <c r="U14" s="12"/>
@@ -2150,7 +2270,6 @@
     <row r="15" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="E15" s="14"/>
-      <c r="F15" s="16"/>
       <c r="G15" s="16"/>
       <c r="M15" s="12"/>
       <c r="N15" s="12"/>
@@ -2177,7 +2296,7 @@
     <row r="16" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="E16" s="14"/>
-      <c r="F16" s="16"/>
+      <c r="F16" s="21"/>
       <c r="G16" s="16"/>
       <c r="M16" s="12"/>
       <c r="N16" s="12"/>
@@ -2285,7 +2404,7 @@
     <row r="20" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="16"/>
+      <c r="F20" s="21"/>
       <c r="G20" s="16"/>
       <c r="M20" s="12"/>
       <c r="N20" s="12"/>
@@ -15323,18 +15442,45 @@
       <c r="AF502" s="12"/>
       <c r="AG502" s="12"/>
     </row>
+    <row r="503" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A503" s="13"/>
+      <c r="E503" s="14"/>
+      <c r="F503" s="16"/>
+      <c r="G503" s="16"/>
+      <c r="M503" s="12"/>
+      <c r="N503" s="12"/>
+      <c r="O503" s="12"/>
+      <c r="P503" s="12"/>
+      <c r="Q503" s="12"/>
+      <c r="R503" s="12"/>
+      <c r="S503" s="17"/>
+      <c r="T503" s="17"/>
+      <c r="U503" s="12"/>
+      <c r="V503" s="12"/>
+      <c r="W503" s="12"/>
+      <c r="X503" s="12"/>
+      <c r="Y503" s="12"/>
+      <c r="Z503" s="13"/>
+      <c r="AA503" s="17"/>
+      <c r="AB503" s="17"/>
+      <c r="AC503" s="12"/>
+      <c r="AD503" s="12"/>
+      <c r="AE503" s="12"/>
+      <c r="AF503" s="12"/>
+      <c r="AG503" s="12"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AA7:AA10 AA13:AA502" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AA14:AA503 AA7:AA11" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Amlodipine,Aspirin,Captopril,Enalpril,Glibenclamide,Glimeperide,Hydrochlorothiazide,Lisinopril,Metformin,Metoprolol,Propranolol"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N3:R502" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N3:R503" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"yes,no,unknown"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D3:D6 D11:D12" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D3:D6 D12:D14" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Male,Female"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E502" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3:E10 E12:E13 E15:E503" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
@@ -15347,13 +15493,13 @@
           <x14:formula1>
             <xm:f>regions!$A$1:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M502</xm:sqref>
+          <xm:sqref>M3:M503</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>'common medicines'!$A$1:$A$40</xm:f>
           </x14:formula1>
-          <xm:sqref>T35:T502 AC3:AG502 U3:Y502</xm:sqref>
+          <xm:sqref>T36:T503 U3:Y503 AC3:AG503</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Skip rows with no reg date
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/patient_import_test.xlsx
+++ b/spec/fixtures/files/patient_import_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hariharanmohanraj/code/simple/simple-server/spec/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FD6B2E-2BA8-214C-8159-306D68BCE5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA640BC-119C-2741-BE85-B6A9675F3221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="155">
   <si>
     <t>registration_date</t>
   </si>
@@ -497,6 +497,9 @@
   <si>
     <t>Random gender</t>
   </si>
+  <si>
+    <t>No Registration Date</t>
+  </si>
 </sst>
 </file>
 
@@ -885,7 +888,7 @@
   <dimension ref="A1:BA503"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2269,6 +2272,9 @@
     </row>
     <row r="15" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
+      <c r="B15" s="14" t="s">
+        <v>154</v>
+      </c>
       <c r="E15" s="14"/>
       <c r="G15" s="16"/>
       <c r="M15" s="12"/>

</xml_diff>